<commit_message>
[fix] update template_exportdb.xlsx for adjust vartical position
</commit_message>
<xml_diff>
--- a/app/FunctionSurvey/management/commands/template_exportdb.xlsx
+++ b/app/FunctionSurvey/management/commands/template_exportdb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc55247\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744ECE69-7449-4153-8D3F-CAA943F4B379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E888D4-19B4-43CB-8AF6-D247B6EF5DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -559,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -577,12 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -999,9 +993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="9.4" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1018,83 +1010,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="17" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="18"/>
+      <c r="G3" s="16"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="19" t="s">
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
     <row r="5" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="19" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="18"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="30" t="s">
+      <c r="C6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="21" t="s">
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="22"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1137,25 +1129,25 @@
       <c r="K9" s="3"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -1185,9 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CF00F3-5BCF-438A-87D1-EC74E4AD1A77}">
   <dimension ref="B1:M11"/>
   <sheetViews>
-    <sheetView zoomScale="111" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView zoomScale="111" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="9.4" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1204,73 +1194,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="14.25" x14ac:dyDescent="0.3">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="38"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="39" t="s">
+      <c r="C3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="40"/>
-      <c r="E3" s="45" t="s">
+      <c r="D3" s="38"/>
+      <c r="E3" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="46"/>
+      <c r="F3" s="44"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="40"/>
+      <c r="E4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="33"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="32" t="s">
+      <c r="D5" s="40"/>
+      <c r="E5" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="33"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="44"/>
-      <c r="E6" s="34" t="s">
+      <c r="D6" s="42"/>
+      <c r="E6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
@@ -1317,34 +1307,34 @@
       <c r="M9" s="3"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="13"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="11"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
[feat] add statement field in funcsurvey
</commit_message>
<xml_diff>
--- a/app/FunctionSurvey/management/commands/template_exportdb.xlsx
+++ b/app/FunctionSurvey/management/commands/template_exportdb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rc55247\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E888D4-19B4-43CB-8AF6-D247B6EF5DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E80CA56B-42B4-4C74-95CA-8769A494E390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -991,9 +991,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:K11"/>
+  <dimension ref="B1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="9.4" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1004,12 +1006,13 @@
     <col min="6" max="6" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.53125" style="1" customWidth="1"/>
     <col min="8" max="8" width="27.73046875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.9296875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="7.53125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.06640625" style="1"/>
+    <col min="9" max="13" width="6.46484375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.9296875" style="1" customWidth="1"/>
+    <col min="15" max="16" width="7.53125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="14.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="14.25" x14ac:dyDescent="0.3">
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1019,7 +1022,7 @@
       <c r="F1" s="14"/>
       <c r="G1" s="14"/>
     </row>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.2">
       <c r="C2" s="21" t="s">
         <v>5</v>
       </c>
@@ -1031,8 +1034,13 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
-    </row>
-    <row r="3" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="26" t="s">
         <v>1</v>
       </c>
@@ -1046,8 +1054,13 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="24" t="s">
         <v>2</v>
       </c>
@@ -1061,8 +1074,13 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="24" t="s">
         <v>3</v>
       </c>
@@ -1076,8 +1094,13 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="2:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="6" spans="2:16" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="28" t="s">
         <v>4</v>
       </c>
@@ -1091,8 +1114,13 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1101,10 +1129,15 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -1113,10 +1146,15 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1127,8 +1165,13 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>11</v>
       </c>
@@ -1141,8 +1184,13 @@
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="11"/>
@@ -1150,9 +1198,14 @@
       <c r="F11" s="11"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>